<commit_message>
-Changed the KT2017 Budget Template
</commit_message>
<xml_diff>
--- a/data/CFN KT2017_Budget.xlsx
+++ b/data/CFN KT2017_Budget.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11130" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10215" tabRatio="677" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Budget Instruction" sheetId="12" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Partner Contributions" sheetId="11" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Budget Summary'!$A$1:$AD$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Budget Summary'!$A$1:$AB$30</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="94">
   <si>
     <t>Foreign</t>
   </si>
@@ -169,9 +169,6 @@
   </si>
   <si>
     <t xml:space="preserve">Discrepancy Check (should be zero) </t>
-  </si>
-  <si>
-    <t>Partner Contributions Total from Summary Tab</t>
   </si>
   <si>
     <t>1.</t>
@@ -300,9 +297,6 @@
     <t>CFN Budget Total:</t>
   </si>
   <si>
-    <t>CFN Budget Total from Summary Tab</t>
-  </si>
-  <si>
     <t>CFN File #:</t>
   </si>
   <si>
@@ -362,6 +356,18 @@
   </si>
   <si>
     <t xml:space="preserve"> 2) CFN Program Budget Summary</t>
+  </si>
+  <si>
+    <t>2019 - 2020 Total</t>
+  </si>
+  <si>
+    <t>Partner Contributions Total from Budget Summary Tab</t>
+  </si>
+  <si>
+    <t>CFN Budget Total from Budget Summary Tab</t>
+  </si>
+  <si>
+    <t>CFN FISCAL YEAR 3 (eg. April 1, 2019 - March 31, 2020)</t>
   </si>
 </sst>
 </file>
@@ -499,7 +505,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -542,6 +548,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="61">
     <border>
@@ -1336,7 +1348,7 @@
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="196">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1581,6 +1593,12 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1634,6 +1652,84 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="15" fontId="3" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1658,74 +1754,17 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="15" fontId="3" fillId="8" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1769,13 +1808,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1831,13 +1870,13 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1850,21 +1889,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2290,8 +2314,8 @@
   </sheetPr>
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:K9"/>
+    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -2681,19 +2705,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="16" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="111" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="113"/>
+      <c r="A1" s="113" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="115"/>
     </row>
     <row r="2" spans="1:13" s="16" customFormat="1" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="94"/>
@@ -2710,18 +2734,18 @@
     </row>
     <row r="3" spans="1:13" s="16" customFormat="1" ht="103.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="94"/>
-      <c r="B3" s="193" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="194"/>
-      <c r="F3" s="194"/>
-      <c r="G3" s="194"/>
-      <c r="H3" s="194"/>
-      <c r="I3" s="194"/>
-      <c r="J3" s="194"/>
-      <c r="K3" s="195"/>
+      <c r="B3" s="130" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="131"/>
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
+      <c r="H3" s="131"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="131"/>
+      <c r="K3" s="132"/>
     </row>
     <row r="4" spans="1:13" s="16" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="93"/>
@@ -2738,80 +2762,80 @@
     </row>
     <row r="5" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="95" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="126" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="126"/>
-      <c r="D5" s="126"/>
-      <c r="E5" s="126"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="126"/>
-      <c r="H5" s="126"/>
-      <c r="I5" s="126"/>
-      <c r="J5" s="126"/>
-      <c r="K5" s="127"/>
+        <v>48</v>
+      </c>
+      <c r="B5" s="128" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="128"/>
+      <c r="D5" s="128"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="128"/>
+      <c r="G5" s="128"/>
+      <c r="H5" s="128"/>
+      <c r="I5" s="128"/>
+      <c r="J5" s="128"/>
+      <c r="K5" s="129"/>
     </row>
     <row r="6" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="96"/>
-      <c r="B6" s="124" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="124"/>
-      <c r="F6" s="124"/>
-      <c r="G6" s="124"/>
-      <c r="H6" s="124"/>
-      <c r="I6" s="124"/>
-      <c r="J6" s="124"/>
-      <c r="K6" s="125"/>
+      <c r="B6" s="126" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="126"/>
+      <c r="D6" s="126"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="126"/>
+      <c r="I6" s="126"/>
+      <c r="J6" s="126"/>
+      <c r="K6" s="127"/>
     </row>
     <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="96"/>
-      <c r="B7" s="124" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="124"/>
-      <c r="D7" s="124"/>
-      <c r="E7" s="124"/>
-      <c r="F7" s="124"/>
-      <c r="G7" s="124"/>
-      <c r="H7" s="124"/>
-      <c r="I7" s="124"/>
-      <c r="J7" s="124"/>
-      <c r="K7" s="125"/>
+      <c r="B7" s="126" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="126"/>
+      <c r="G7" s="126"/>
+      <c r="H7" s="126"/>
+      <c r="I7" s="126"/>
+      <c r="J7" s="126"/>
+      <c r="K7" s="127"/>
     </row>
     <row r="8" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="96"/>
-      <c r="B8" s="124" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="124"/>
-      <c r="D8" s="124"/>
-      <c r="E8" s="124"/>
-      <c r="F8" s="124"/>
-      <c r="G8" s="124"/>
-      <c r="H8" s="124"/>
-      <c r="I8" s="124"/>
-      <c r="J8" s="124"/>
-      <c r="K8" s="125"/>
+      <c r="B8" s="126" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="126"/>
+      <c r="D8" s="126"/>
+      <c r="E8" s="126"/>
+      <c r="F8" s="126"/>
+      <c r="G8" s="126"/>
+      <c r="H8" s="126"/>
+      <c r="I8" s="126"/>
+      <c r="J8" s="126"/>
+      <c r="K8" s="127"/>
     </row>
     <row r="9" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="97"/>
-      <c r="B9" s="122" t="s">
+      <c r="B9" s="124" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="122"/>
-      <c r="D9" s="122"/>
-      <c r="E9" s="122"/>
-      <c r="F9" s="122"/>
-      <c r="G9" s="122"/>
-      <c r="H9" s="122"/>
-      <c r="I9" s="122"/>
-      <c r="J9" s="122"/>
-      <c r="K9" s="123"/>
+      <c r="C9" s="124"/>
+      <c r="D9" s="124"/>
+      <c r="E9" s="124"/>
+      <c r="F9" s="124"/>
+      <c r="G9" s="124"/>
+      <c r="H9" s="124"/>
+      <c r="I9" s="124"/>
+      <c r="J9" s="124"/>
+      <c r="K9" s="125"/>
       <c r="M9" s="109"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
@@ -2829,20 +2853,20 @@
     </row>
     <row r="11" spans="1:13" ht="69" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="99" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="120" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="120"/>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
-      <c r="G11" s="120"/>
-      <c r="H11" s="120"/>
-      <c r="I11" s="120"/>
-      <c r="J11" s="120"/>
-      <c r="K11" s="121"/>
+        <v>49</v>
+      </c>
+      <c r="B11" s="122" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="122"/>
+      <c r="D11" s="122"/>
+      <c r="E11" s="122"/>
+      <c r="F11" s="122"/>
+      <c r="G11" s="122"/>
+      <c r="H11" s="122"/>
+      <c r="I11" s="122"/>
+      <c r="J11" s="122"/>
+      <c r="K11" s="123"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="98"/>
@@ -2859,20 +2883,20 @@
     </row>
     <row r="13" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="99" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="120" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="120"/>
-      <c r="D13" s="120"/>
-      <c r="E13" s="120"/>
-      <c r="F13" s="120"/>
-      <c r="G13" s="120"/>
-      <c r="H13" s="120"/>
-      <c r="I13" s="120"/>
-      <c r="J13" s="120"/>
-      <c r="K13" s="121"/>
+        <v>50</v>
+      </c>
+      <c r="B13" s="122" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="122"/>
+      <c r="D13" s="122"/>
+      <c r="E13" s="122"/>
+      <c r="F13" s="122"/>
+      <c r="G13" s="122"/>
+      <c r="H13" s="122"/>
+      <c r="I13" s="122"/>
+      <c r="J13" s="122"/>
+      <c r="K13" s="123"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="98"/>
@@ -2889,10 +2913,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="95" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="100" t="s">
         <v>52</v>
-      </c>
-      <c r="B15" s="100" t="s">
-        <v>53</v>
       </c>
       <c r="C15" s="100"/>
       <c r="D15" s="100"/>
@@ -2906,48 +2930,48 @@
     </row>
     <row r="16" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="96"/>
-      <c r="B16" s="114" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="114"/>
-      <c r="D16" s="114"/>
-      <c r="E16" s="114"/>
-      <c r="F16" s="114"/>
-      <c r="G16" s="114"/>
-      <c r="H16" s="114"/>
-      <c r="I16" s="114"/>
-      <c r="J16" s="114"/>
-      <c r="K16" s="115"/>
+      <c r="B16" s="116" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="116"/>
+      <c r="G16" s="116"/>
+      <c r="H16" s="116"/>
+      <c r="I16" s="116"/>
+      <c r="J16" s="116"/>
+      <c r="K16" s="117"/>
     </row>
     <row r="17" spans="1:11" ht="71.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="96"/>
-      <c r="B17" s="116" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="116"/>
-      <c r="D17" s="116"/>
-      <c r="E17" s="116"/>
-      <c r="F17" s="116"/>
-      <c r="G17" s="116"/>
-      <c r="H17" s="116"/>
-      <c r="I17" s="116"/>
-      <c r="J17" s="116"/>
-      <c r="K17" s="117"/>
+      <c r="B17" s="118" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="118"/>
+      <c r="D17" s="118"/>
+      <c r="E17" s="118"/>
+      <c r="F17" s="118"/>
+      <c r="G17" s="118"/>
+      <c r="H17" s="118"/>
+      <c r="I17" s="118"/>
+      <c r="J17" s="118"/>
+      <c r="K17" s="119"/>
     </row>
     <row r="18" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="97"/>
-      <c r="B18" s="118" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="118"/>
-      <c r="D18" s="118"/>
-      <c r="E18" s="118"/>
-      <c r="F18" s="118"/>
-      <c r="G18" s="118"/>
-      <c r="H18" s="118"/>
-      <c r="I18" s="118"/>
-      <c r="J18" s="118"/>
-      <c r="K18" s="119"/>
+      <c r="B18" s="120" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="120"/>
+      <c r="D18" s="120"/>
+      <c r="E18" s="120"/>
+      <c r="F18" s="120"/>
+      <c r="G18" s="120"/>
+      <c r="H18" s="120"/>
+      <c r="I18" s="120"/>
+      <c r="J18" s="120"/>
+      <c r="K18" s="121"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B19" s="90"/>
@@ -3054,36 +3078,36 @@
     <tabColor rgb="FFC00000"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AJ30"/>
+  <dimension ref="A1:AH30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.1328125" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
-    <col min="3" max="23" width="10.265625" style="1" customWidth="1"/>
-    <col min="24" max="25" width="11.73046875" style="1" customWidth="1"/>
-    <col min="26" max="26" width="5.73046875" style="1" customWidth="1"/>
-    <col min="27" max="27" width="5.73046875" customWidth="1"/>
-    <col min="28" max="237" width="5.73046875" style="1" customWidth="1"/>
-    <col min="238" max="16384" width="1.1328125" style="1"/>
+    <col min="3" max="21" width="10.265625" style="1" customWidth="1"/>
+    <col min="22" max="23" width="11.73046875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="11" style="1" customWidth="1"/>
+    <col min="25" max="25" width="12.3984375" customWidth="1"/>
+    <col min="26" max="235" width="5.73046875" style="1" customWidth="1"/>
+    <col min="236" max="16384" width="1.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="154" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="154"/>
-      <c r="D1" s="154"/>
-      <c r="E1" s="154"/>
-      <c r="F1" s="154"/>
-      <c r="G1" s="154"/>
-      <c r="H1" s="154"/>
-      <c r="I1" s="154"/>
+    <row r="1" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="138" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="138"/>
+      <c r="C1" s="138"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
       <c r="J1" s="106"/>
       <c r="K1" s="106"/>
       <c r="L1" s="106"/>
@@ -3096,23 +3120,21 @@
       <c r="S1" s="106"/>
       <c r="T1" s="106"/>
       <c r="U1" s="106"/>
-      <c r="V1" s="106"/>
-      <c r="W1" s="106"/>
-    </row>
-    <row r="2" spans="1:36" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="149" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="150"/>
-      <c r="C2" s="151" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="152"/>
-      <c r="E2" s="152"/>
-      <c r="F2" s="152"/>
-      <c r="G2" s="152"/>
-      <c r="H2" s="152"/>
-      <c r="I2" s="153"/>
+    </row>
+    <row r="2" spans="1:34" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="133" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="134"/>
+      <c r="C2" s="135" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="137"/>
       <c r="J2" s="107"/>
       <c r="K2" s="107"/>
       <c r="L2" s="107"/>
@@ -3125,24 +3147,22 @@
       <c r="S2" s="107"/>
       <c r="T2" s="107"/>
       <c r="U2" s="107"/>
-      <c r="V2" s="107"/>
-      <c r="W2" s="107"/>
-      <c r="Z2" s="8"/>
-    </row>
-    <row r="3" spans="1:36" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="149" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="150"/>
-      <c r="C3" s="151" t="s">
+      <c r="X2" s="8"/>
+    </row>
+    <row r="3" spans="1:34" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="133" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="134"/>
+      <c r="C3" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="152"/>
-      <c r="E3" s="152"/>
-      <c r="F3" s="152"/>
-      <c r="G3" s="152"/>
-      <c r="H3" s="152"/>
-      <c r="I3" s="153"/>
+      <c r="D3" s="136"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="136"/>
+      <c r="H3" s="136"/>
+      <c r="I3" s="137"/>
       <c r="J3" s="107"/>
       <c r="K3" s="107"/>
       <c r="L3" s="107"/>
@@ -3155,24 +3175,22 @@
       <c r="S3" s="107"/>
       <c r="T3" s="107"/>
       <c r="U3" s="107"/>
-      <c r="V3" s="107"/>
-      <c r="W3" s="107"/>
-      <c r="Z3" s="8"/>
-    </row>
-    <row r="4" spans="1:36" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="155" t="s">
-        <v>83</v>
-      </c>
-      <c r="B4" s="155"/>
-      <c r="C4" s="151" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="152"/>
-      <c r="E4" s="152"/>
-      <c r="F4" s="152"/>
-      <c r="G4" s="152"/>
-      <c r="H4" s="152"/>
-      <c r="I4" s="153"/>
+      <c r="X3" s="8"/>
+    </row>
+    <row r="4" spans="1:34" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="139" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="139"/>
+      <c r="C4" s="135" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="137"/>
       <c r="J4" s="107"/>
       <c r="K4" s="107"/>
       <c r="L4" s="107"/>
@@ -3185,24 +3203,22 @@
       <c r="S4" s="107"/>
       <c r="T4" s="107"/>
       <c r="U4" s="107"/>
-      <c r="V4" s="107"/>
-      <c r="W4" s="107"/>
-      <c r="Z4" s="8"/>
-    </row>
-    <row r="5" spans="1:36" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="155" t="s">
+      <c r="X4" s="8"/>
+    </row>
+    <row r="5" spans="1:34" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="139" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="155"/>
-      <c r="C5" s="151" t="s">
+      <c r="B5" s="139"/>
+      <c r="C5" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="152"/>
-      <c r="E5" s="152"/>
-      <c r="F5" s="152"/>
-      <c r="G5" s="152"/>
-      <c r="H5" s="152"/>
-      <c r="I5" s="153"/>
+      <c r="D5" s="136"/>
+      <c r="E5" s="136"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
+      <c r="H5" s="136"/>
+      <c r="I5" s="137"/>
       <c r="J5" s="107"/>
       <c r="K5" s="107"/>
       <c r="L5" s="107"/>
@@ -3215,24 +3231,22 @@
       <c r="S5" s="107"/>
       <c r="T5" s="107"/>
       <c r="U5" s="107"/>
-      <c r="V5" s="107"/>
-      <c r="W5" s="107"/>
-      <c r="Z5" s="8"/>
-    </row>
-    <row r="6" spans="1:36" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="155" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="155"/>
-      <c r="C6" s="151" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="152"/>
-      <c r="E6" s="152"/>
-      <c r="F6" s="152"/>
-      <c r="G6" s="152"/>
-      <c r="H6" s="152"/>
-      <c r="I6" s="153"/>
+      <c r="X5" s="8"/>
+    </row>
+    <row r="6" spans="1:34" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="139" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="139"/>
+      <c r="C6" s="135" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="136"/>
+      <c r="E6" s="136"/>
+      <c r="F6" s="136"/>
+      <c r="G6" s="136"/>
+      <c r="H6" s="136"/>
+      <c r="I6" s="137"/>
       <c r="J6" s="107"/>
       <c r="K6" s="107"/>
       <c r="L6" s="107"/>
@@ -3245,11 +3259,9 @@
       <c r="S6" s="107"/>
       <c r="T6" s="107"/>
       <c r="U6" s="107"/>
-      <c r="V6" s="107"/>
-      <c r="W6" s="107"/>
-      <c r="Z6" s="6"/>
-    </row>
-    <row r="7" spans="1:36" s="2" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="X6" s="6"/>
+    </row>
+    <row r="7" spans="1:34" s="2" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -3267,78 +3279,94 @@
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="Z7" s="6"/>
-    </row>
-    <row r="8" spans="1:36" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="X7" s="6"/>
+    </row>
+    <row r="8" spans="1:34" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="17"/>
-      <c r="C8" s="128" t="s">
+      <c r="C8" s="155" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="156"/>
+      <c r="E8" s="156"/>
+      <c r="F8" s="156"/>
+      <c r="G8" s="156"/>
+      <c r="H8" s="156"/>
+      <c r="I8" s="157"/>
+      <c r="J8" s="158" t="s">
+        <v>78</v>
+      </c>
+      <c r="K8" s="159"/>
+      <c r="L8" s="159"/>
+      <c r="M8" s="159"/>
+      <c r="N8" s="159"/>
+      <c r="O8" s="159"/>
+      <c r="P8" s="160"/>
+      <c r="Q8" s="161" t="s">
+        <v>93</v>
+      </c>
+      <c r="R8" s="162"/>
+      <c r="S8" s="162"/>
+      <c r="T8" s="162"/>
+      <c r="U8" s="162"/>
+      <c r="V8" s="162"/>
+      <c r="W8" s="163"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+    </row>
+    <row r="9" spans="1:34" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="144" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="145"/>
+      <c r="C9" s="149" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="150"/>
+      <c r="E9" s="150"/>
+      <c r="F9" s="146" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="147"/>
+      <c r="H9" s="148"/>
+      <c r="I9" s="141" t="s">
+        <v>80</v>
+      </c>
+      <c r="J9" s="149" t="s">
+        <v>70</v>
+      </c>
+      <c r="K9" s="150"/>
+      <c r="L9" s="150"/>
+      <c r="M9" s="146" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" s="147"/>
+      <c r="O9" s="148"/>
+      <c r="P9" s="141" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="129"/>
-      <c r="E8" s="129"/>
-      <c r="F8" s="129"/>
-      <c r="G8" s="129"/>
-      <c r="H8" s="129"/>
-      <c r="I8" s="130"/>
-      <c r="J8" s="131" t="s">
-        <v>80</v>
-      </c>
-      <c r="K8" s="132"/>
-      <c r="L8" s="132"/>
-      <c r="M8" s="132"/>
-      <c r="N8" s="132"/>
-      <c r="O8" s="132"/>
-      <c r="P8" s="133"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8"/>
-      <c r="AA8" s="1"/>
-    </row>
-    <row r="9" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="142" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="143"/>
-      <c r="C9" s="147" t="s">
+      <c r="Q9" s="149" t="s">
+        <v>70</v>
+      </c>
+      <c r="R9" s="150"/>
+      <c r="S9" s="150"/>
+      <c r="T9" s="146" t="s">
+        <v>17</v>
+      </c>
+      <c r="U9" s="147"/>
+      <c r="V9" s="148"/>
+      <c r="W9" s="141" t="s">
+        <v>90</v>
+      </c>
+      <c r="X9" s="151" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="148"/>
-      <c r="E9" s="148"/>
-      <c r="F9" s="144" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="145"/>
-      <c r="H9" s="146"/>
-      <c r="I9" s="135" t="s">
-        <v>82</v>
-      </c>
-      <c r="J9" s="147" t="s">
-        <v>71</v>
-      </c>
-      <c r="K9" s="148"/>
-      <c r="L9" s="148"/>
-      <c r="M9" s="144" t="s">
-        <v>17</v>
-      </c>
-      <c r="N9" s="145"/>
-      <c r="O9" s="146"/>
-      <c r="P9" s="135" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q9" s="137" t="s">
+      <c r="Y9" s="153" t="s">
         <v>72</v>
       </c>
-      <c r="R9" s="139" t="s">
-        <v>73</v>
-      </c>
-      <c r="S9"/>
-      <c r="AA9" s="1"/>
-      <c r="AJ9" s="3"/>
-    </row>
-    <row r="10" spans="1:36" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="AH9" s="3"/>
+    </row>
+    <row r="10" spans="1:34" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A10" s="67" t="s">
         <v>21</v>
       </c>
@@ -3363,7 +3391,7 @@
       <c r="H10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="136"/>
+      <c r="I10" s="142"/>
       <c r="J10" s="80" t="s">
         <v>8</v>
       </c>
@@ -3382,14 +3410,31 @@
       <c r="O10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="P10" s="136"/>
-      <c r="Q10" s="138"/>
-      <c r="R10" s="140"/>
-      <c r="S10"/>
-      <c r="AA10" s="1"/>
-      <c r="AJ10" s="3"/>
-    </row>
-    <row r="11" spans="1:36" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="P10" s="142"/>
+      <c r="Q10" s="80" t="s">
+        <v>8</v>
+      </c>
+      <c r="R10" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="S10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="T10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="U10" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="V10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="W10" s="142"/>
+      <c r="X10" s="152"/>
+      <c r="Y10" s="154"/>
+      <c r="AH10" s="3"/>
+    </row>
+    <row r="11" spans="1:34" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
         <v>1</v>
       </c>
@@ -3408,12 +3453,17 @@
       <c r="N11" s="22"/>
       <c r="O11" s="22"/>
       <c r="P11" s="28"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="30"/>
-      <c r="S11"/>
-      <c r="AA11" s="1"/>
-    </row>
-    <row r="12" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q11" s="25"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="18"/>
+      <c r="T11" s="18"/>
+      <c r="U11" s="22"/>
+      <c r="V11" s="22"/>
+      <c r="W11" s="28"/>
+      <c r="X11" s="29"/>
+      <c r="Y11" s="30"/>
+    </row>
+    <row r="12" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
         <v>2</v>
       </c>
@@ -3450,18 +3500,32 @@
         <f>L12+O12</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="32">
-        <f>E12+L12</f>
-        <v>0</v>
-      </c>
-      <c r="R12" s="38">
-        <f>I12+P12</f>
-        <v>0</v>
-      </c>
-      <c r="S12"/>
-      <c r="AA12" s="1"/>
-    </row>
-    <row r="13" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q12" s="81"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="32">
+        <f>SUM(Q12:R12)</f>
+        <v>0</v>
+      </c>
+      <c r="T12" s="34"/>
+      <c r="U12" s="86"/>
+      <c r="V12" s="37">
+        <f>SUM(T12:U12)</f>
+        <v>0</v>
+      </c>
+      <c r="W12" s="38">
+        <f>S12+V12</f>
+        <v>0</v>
+      </c>
+      <c r="X12" s="32">
+        <f>E12+L12+S12</f>
+        <v>0</v>
+      </c>
+      <c r="Y12" s="38">
+        <f>I12+P12+W12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
         <v>3</v>
       </c>
@@ -3498,18 +3562,32 @@
         <f>L13+O13</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="32">
-        <f t="shared" ref="Q13:Q14" si="0">E13+L13</f>
-        <v>0</v>
-      </c>
-      <c r="R13" s="38">
-        <f t="shared" ref="R13:R14" si="1">I13+P13</f>
-        <v>0</v>
-      </c>
-      <c r="S13"/>
-      <c r="AA13" s="1"/>
-    </row>
-    <row r="14" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q13" s="82"/>
+      <c r="R13" s="33"/>
+      <c r="S13" s="32">
+        <f>SUM(Q13:R13)</f>
+        <v>0</v>
+      </c>
+      <c r="T13" s="33"/>
+      <c r="U13" s="87"/>
+      <c r="V13" s="40">
+        <f>SUM(T13:U13)</f>
+        <v>0</v>
+      </c>
+      <c r="W13" s="38">
+        <f>S13+V13</f>
+        <v>0</v>
+      </c>
+      <c r="X13" s="32">
+        <f>E13+L13+S13</f>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="38">
+        <f>I13+P13+W13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>4</v>
       </c>
@@ -3546,18 +3624,32 @@
         <f>L14+O14</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R14" s="38">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S14"/>
-      <c r="AA14" s="1"/>
-    </row>
-    <row r="15" spans="1:36" ht="20.65" x14ac:dyDescent="0.35">
+      <c r="Q14" s="82"/>
+      <c r="R14" s="33"/>
+      <c r="S14" s="32">
+        <f>SUM(Q14:R14)</f>
+        <v>0</v>
+      </c>
+      <c r="T14" s="34"/>
+      <c r="U14" s="86"/>
+      <c r="V14" s="37">
+        <f>SUM(T14:U14)</f>
+        <v>0</v>
+      </c>
+      <c r="W14" s="38">
+        <f>S14+V14</f>
+        <v>0</v>
+      </c>
+      <c r="X14" s="32">
+        <f>E14+L14+S14</f>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="38">
+        <f>I14+P14+W14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
         <v>5</v>
       </c>
@@ -3576,12 +3668,17 @@
       <c r="N15" s="23"/>
       <c r="O15" s="23"/>
       <c r="P15" s="27"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="27"/>
-      <c r="S15"/>
-      <c r="AA15" s="1"/>
-    </row>
-    <row r="16" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q15" s="83"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="27"/>
+      <c r="X15" s="24"/>
+      <c r="Y15" s="27"/>
+    </row>
+    <row r="16" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="s">
         <v>6</v>
       </c>
@@ -3618,18 +3715,32 @@
         <f>L16+O16</f>
         <v>0</v>
       </c>
-      <c r="Q16" s="32">
-        <f>E16+L16</f>
-        <v>0</v>
-      </c>
-      <c r="R16" s="38">
-        <f>I16+P16</f>
-        <v>0</v>
-      </c>
-      <c r="S16"/>
-      <c r="AA16" s="1"/>
-    </row>
-    <row r="17" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q16" s="82"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="32">
+        <f>SUM(Q16:R16)</f>
+        <v>0</v>
+      </c>
+      <c r="T16" s="34"/>
+      <c r="U16" s="36"/>
+      <c r="V16" s="37">
+        <f>SUM(T16:U16)</f>
+        <v>0</v>
+      </c>
+      <c r="W16" s="38">
+        <f>S16+V16</f>
+        <v>0</v>
+      </c>
+      <c r="X16" s="32">
+        <f t="shared" ref="X16:X23" si="0">E16+L16+S16</f>
+        <v>0</v>
+      </c>
+      <c r="Y16" s="38">
+        <f t="shared" ref="Y16:Y23" si="1">I16+P16+W16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
         <v>20</v>
       </c>
@@ -3666,90 +3777,130 @@
         <f>L17+O17</f>
         <v>0</v>
       </c>
-      <c r="Q17" s="32">
-        <f t="shared" ref="Q17:Q22" si="2">E17+L17</f>
-        <v>0</v>
-      </c>
-      <c r="R17" s="38">
-        <f t="shared" ref="R17:R22" si="3">I17+P17</f>
-        <v>0</v>
-      </c>
-      <c r="S17"/>
-      <c r="AA17" s="1"/>
-    </row>
-    <row r="18" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q17" s="82"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="32">
+        <f>SUM(Q17:R17)</f>
+        <v>0</v>
+      </c>
+      <c r="T17" s="34"/>
+      <c r="U17" s="36"/>
+      <c r="V17" s="37">
+        <f>SUM(T17:U17)</f>
+        <v>0</v>
+      </c>
+      <c r="W17" s="38">
+        <f>S17+V17</f>
+        <v>0</v>
+      </c>
+      <c r="X17" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y17" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="26" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="77"/>
       <c r="C18" s="84">
-        <f t="shared" ref="C18:N18" si="4">SUM(C12:C17)</f>
+        <f t="shared" ref="C18:N18" si="2">SUM(C12:C17)</f>
         <v>0</v>
       </c>
       <c r="D18" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E18" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F18" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G18" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H18" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I18" s="42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J18" s="84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K18" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L18" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M18" s="35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N18" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O18" s="41">
-        <f t="shared" ref="O18" si="5">SUM(O12:O17)</f>
+        <f t="shared" ref="O18" si="3">SUM(O12:O17)</f>
         <v>0</v>
       </c>
       <c r="P18" s="42">
-        <f t="shared" ref="P18" si="6">SUM(P12:P17)</f>
-        <v>0</v>
-      </c>
-      <c r="Q18" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R18" s="38">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S18"/>
-      <c r="AA18" s="1"/>
-    </row>
-    <row r="19" spans="1:27" ht="20.65" x14ac:dyDescent="0.35">
+        <f t="shared" ref="P18" si="4">SUM(P12:P17)</f>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="84">
+        <f t="shared" ref="Q18:W18" si="5">SUM(Q12:Q17)</f>
+        <v>0</v>
+      </c>
+      <c r="R18" s="35">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S18" s="35">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T18" s="35">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U18" s="41">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V18" s="41">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="W18" s="42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="X18" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y18" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A19" s="26" t="s">
         <v>13</v>
       </c>
@@ -3786,18 +3937,32 @@
         <f>L19+O19</f>
         <v>0</v>
       </c>
-      <c r="Q19" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R19" s="38">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S19"/>
-      <c r="AA19" s="1"/>
-    </row>
-    <row r="20" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q19" s="82"/>
+      <c r="R19" s="34"/>
+      <c r="S19" s="32">
+        <f>SUM(Q19:R19)</f>
+        <v>0</v>
+      </c>
+      <c r="T19" s="33"/>
+      <c r="U19" s="39"/>
+      <c r="V19" s="40">
+        <f>SUM(T19:U19)</f>
+        <v>0</v>
+      </c>
+      <c r="W19" s="38">
+        <f>S19+V19</f>
+        <v>0</v>
+      </c>
+      <c r="X19" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y19" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
         <v>22</v>
       </c>
@@ -3834,18 +3999,32 @@
         <f>L20+O20</f>
         <v>0</v>
       </c>
-      <c r="Q20" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R20" s="38">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S20"/>
-      <c r="AA20" s="1"/>
-    </row>
-    <row r="21" spans="1:27" ht="20.65" x14ac:dyDescent="0.35">
+      <c r="Q20" s="82"/>
+      <c r="R20" s="34"/>
+      <c r="S20" s="32">
+        <f>SUM(Q20:R20)</f>
+        <v>0</v>
+      </c>
+      <c r="T20" s="34"/>
+      <c r="U20" s="36"/>
+      <c r="V20" s="37">
+        <f>SUM(T20:U20)</f>
+        <v>0</v>
+      </c>
+      <c r="W20" s="38">
+        <f>S20+V20</f>
+        <v>0</v>
+      </c>
+      <c r="X20" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y20" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A21" s="26" t="s">
         <v>14</v>
       </c>
@@ -3882,18 +4061,32 @@
         <f>L21+O21</f>
         <v>0</v>
       </c>
-      <c r="Q21" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R21" s="38">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S21"/>
-      <c r="AA21" s="1"/>
-    </row>
-    <row r="22" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q21" s="82"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="32">
+        <f>SUM(Q21:R21)</f>
+        <v>0</v>
+      </c>
+      <c r="T21" s="34"/>
+      <c r="U21" s="36"/>
+      <c r="V21" s="37">
+        <f>SUM(T21:U21)</f>
+        <v>0</v>
+      </c>
+      <c r="W21" s="38">
+        <f>S21+V21</f>
+        <v>0</v>
+      </c>
+      <c r="X21" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y21" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="s">
         <v>23</v>
       </c>
@@ -3930,18 +4123,32 @@
         <f>L22+O22</f>
         <v>0</v>
       </c>
-      <c r="Q22" s="32">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R22" s="38">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S22"/>
-      <c r="AA22" s="1"/>
-    </row>
-    <row r="23" spans="1:27" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q22" s="82"/>
+      <c r="R22" s="34"/>
+      <c r="S22" s="32">
+        <f>SUM(Q22:R22)</f>
+        <v>0</v>
+      </c>
+      <c r="T22" s="34"/>
+      <c r="U22" s="36"/>
+      <c r="V22" s="37">
+        <f>SUM(T22:U22)</f>
+        <v>0</v>
+      </c>
+      <c r="W22" s="38">
+        <f>S22+V22</f>
+        <v>0</v>
+      </c>
+      <c r="X22" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y22" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="68" t="s">
         <v>19</v>
       </c>
@@ -3970,134 +4177,173 @@
         <v>0</v>
       </c>
       <c r="H23" s="71">
-        <f t="shared" ref="H23" si="7">SUM(H18:H22)</f>
+        <f t="shared" ref="H23" si="6">SUM(H18:H22)</f>
         <v>0</v>
       </c>
       <c r="I23" s="72">
-        <f t="shared" ref="I23:R23" si="8">SUM(I18:I22)</f>
+        <f t="shared" ref="I23:P23" si="7">SUM(I18:I22)</f>
         <v>0</v>
       </c>
       <c r="J23" s="85">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="69">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L23" s="70">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="69">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="71">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O23" s="71">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P23" s="72">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="85">
+        <f t="shared" ref="Q23:W23" si="8">SUM(Q18:Q22)</f>
+        <v>0</v>
+      </c>
+      <c r="R23" s="69">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="K23" s="69">
+      <c r="S23" s="70">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="L23" s="70">
+      <c r="T23" s="69">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="M23" s="69">
+      <c r="U23" s="71">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N23" s="71">
+      <c r="V23" s="71">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="O23" s="71">
+      <c r="W23" s="72">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="P23" s="72">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="72">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="R23" s="72">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="S23"/>
-      <c r="AA23" s="1"/>
-    </row>
-    <row r="24" spans="1:27" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X23" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y23" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="89"/>
-      <c r="AA24" s="1"/>
-    </row>
-    <row r="25" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="141" t="s">
-        <v>74</v>
-      </c>
-      <c r="B25" s="141"/>
-      <c r="C25" s="141"/>
-      <c r="D25" s="141"/>
-      <c r="E25" s="141"/>
-      <c r="F25" s="141"/>
-      <c r="G25" s="141"/>
-      <c r="H25" s="141"/>
-      <c r="I25" s="141"/>
-      <c r="J25" s="141"/>
-      <c r="K25" s="141"/>
-      <c r="L25" s="141"/>
-      <c r="M25" s="141"/>
-      <c r="N25" s="141"/>
-      <c r="O25" s="141"/>
-      <c r="P25" s="141"/>
-      <c r="Q25" s="141"/>
-      <c r="R25" s="141"/>
-      <c r="S25" s="141"/>
-      <c r="T25" s="141"/>
-      <c r="U25" s="141"/>
-      <c r="V25" s="141"/>
-      <c r="W25" s="141"/>
-      <c r="X25" s="141"/>
-      <c r="Y25" s="141"/>
-      <c r="AA25" s="1"/>
-    </row>
-    <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="134" t="s">
-        <v>85</v>
-      </c>
-      <c r="B26" s="134"/>
-      <c r="C26" s="134"/>
-      <c r="D26" s="134"/>
-      <c r="E26" s="134"/>
-      <c r="F26" s="134"/>
-      <c r="G26" s="134"/>
-      <c r="H26" s="134"/>
-      <c r="I26" s="134"/>
-      <c r="J26" s="134"/>
-      <c r="K26" s="134"/>
-      <c r="L26" s="134"/>
-      <c r="M26" s="134"/>
-      <c r="N26" s="134"/>
-      <c r="O26" s="134"/>
-      <c r="P26" s="134"/>
-      <c r="Q26" s="134"/>
-      <c r="R26" s="134"/>
-      <c r="S26" s="134"/>
-      <c r="T26" s="134"/>
-      <c r="U26" s="134"/>
-      <c r="V26" s="134"/>
-      <c r="W26" s="134"/>
-      <c r="X26" s="134"/>
-      <c r="Y26" s="134"/>
-      <c r="AA26" s="1"/>
-    </row>
-    <row r="27" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Y27" s="2"/>
-      <c r="AA27" s="1"/>
-    </row>
-    <row r="28" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Y28" s="2"/>
-      <c r="AA28" s="1"/>
-    </row>
-    <row r="29" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Y29" s="2"/>
-      <c r="AA29" s="1"/>
-    </row>
-    <row r="30" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Y30" s="2"/>
-      <c r="AA30" s="1"/>
+      <c r="Y24" s="1"/>
+    </row>
+    <row r="25" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="143" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="143"/>
+      <c r="C25" s="143"/>
+      <c r="D25" s="143"/>
+      <c r="E25" s="143"/>
+      <c r="F25" s="143"/>
+      <c r="G25" s="143"/>
+      <c r="H25" s="143"/>
+      <c r="I25" s="143"/>
+      <c r="J25" s="143"/>
+      <c r="K25" s="143"/>
+      <c r="L25" s="143"/>
+      <c r="M25" s="143"/>
+      <c r="N25" s="143"/>
+      <c r="O25" s="143"/>
+      <c r="P25" s="143"/>
+      <c r="Q25" s="143"/>
+      <c r="R25" s="143"/>
+      <c r="S25" s="143"/>
+      <c r="T25" s="143"/>
+      <c r="U25" s="143"/>
+      <c r="V25" s="143"/>
+      <c r="W25" s="143"/>
+      <c r="Y25" s="1"/>
+    </row>
+    <row r="26" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="140" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="140"/>
+      <c r="C26" s="140"/>
+      <c r="D26" s="140"/>
+      <c r="E26" s="140"/>
+      <c r="F26" s="140"/>
+      <c r="G26" s="140"/>
+      <c r="H26" s="140"/>
+      <c r="I26" s="140"/>
+      <c r="J26" s="140"/>
+      <c r="K26" s="140"/>
+      <c r="L26" s="140"/>
+      <c r="M26" s="140"/>
+      <c r="N26" s="140"/>
+      <c r="O26" s="140"/>
+      <c r="P26" s="140"/>
+      <c r="Q26" s="140"/>
+      <c r="R26" s="140"/>
+      <c r="S26" s="140"/>
+      <c r="T26" s="140"/>
+      <c r="U26" s="140"/>
+      <c r="V26" s="140"/>
+      <c r="W26" s="140"/>
+      <c r="Y26" s="1"/>
+    </row>
+    <row r="27" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W27" s="2"/>
+      <c r="Y27" s="1"/>
+    </row>
+    <row r="28" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W28" s="2"/>
+      <c r="Y28" s="1"/>
+    </row>
+    <row r="29" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W29" s="2"/>
+      <c r="Y29" s="1"/>
+    </row>
+    <row r="30" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W30" s="2"/>
+      <c r="Y30" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="28">
+    <mergeCell ref="X9:X10"/>
+    <mergeCell ref="Y9:Y10"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="J8:P8"/>
+    <mergeCell ref="Q8:W8"/>
+    <mergeCell ref="A26:W26"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="A25:W25"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="T9:V9"/>
+    <mergeCell ref="W9:W10"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="A1:I1"/>
@@ -4109,19 +4355,6 @@
     <mergeCell ref="C5:I5"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="J8:P8"/>
-    <mergeCell ref="A26:Y26"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="A25:Y25"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="P9:P10"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions gridLines="1"/>
@@ -4133,6 +4366,9 @@
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="30" max="21" man="1"/>
   </rowBreaks>
+  <ignoredErrors>
+    <ignoredError sqref="E18 H18:I18 L18 O18:P18 S18 V18:W18" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -4145,7 +4381,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E4"/>
+      <selection activeCell="A21" sqref="A21:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -4536,70 +4772,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="10" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="165" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="167"/>
+      <c r="A1" s="173" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="175"/>
       <c r="F1" s="9"/>
       <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="157"/>
+        <v>69</v>
+      </c>
+      <c r="B2" s="184"/>
+      <c r="C2" s="164"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="165"/>
       <c r="I2" s="16"/>
     </row>
     <row r="3" spans="1:10" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="151" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="156"/>
-      <c r="D3" s="156"/>
-      <c r="E3" s="157"/>
+      <c r="B3" s="135" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="164"/>
+      <c r="D3" s="164"/>
+      <c r="E3" s="165"/>
       <c r="F3" s="13"/>
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:10" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="51" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" s="176"/>
-      <c r="C4" s="156"/>
-      <c r="D4" s="156"/>
-      <c r="E4" s="157"/>
+        <v>84</v>
+      </c>
+      <c r="B4" s="184"/>
+      <c r="C4" s="164"/>
+      <c r="D4" s="164"/>
+      <c r="E4" s="165"/>
       <c r="I4" s="16"/>
     </row>
     <row r="5" spans="1:10" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="176" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="156"/>
-      <c r="D5" s="156"/>
-      <c r="E5" s="157"/>
+      <c r="B5" s="184" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="164"/>
+      <c r="D5" s="164"/>
+      <c r="E5" s="165"/>
       <c r="F5" s="13"/>
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:10" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="174"/>
-      <c r="C6" s="174"/>
-      <c r="D6" s="174"/>
-      <c r="E6" s="175"/>
+        <v>61</v>
+      </c>
+      <c r="B6" s="182"/>
+      <c r="C6" s="182"/>
+      <c r="D6" s="182"/>
+      <c r="E6" s="183"/>
       <c r="I6" s="16"/>
     </row>
     <row r="7" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.4">
@@ -4715,13 +4951,13 @@
       </c>
     </row>
     <row r="16" spans="1:10" s="16" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="171" t="s">
+      <c r="A16" s="179" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="172"/>
-      <c r="C16" s="172"/>
-      <c r="D16" s="172"/>
-      <c r="E16" s="173"/>
+      <c r="B16" s="180"/>
+      <c r="C16" s="180"/>
+      <c r="D16" s="180"/>
+      <c r="E16" s="181"/>
     </row>
     <row r="17" spans="1:5" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="62" t="s">
@@ -4784,13 +5020,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" s="16" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="171" t="s">
+      <c r="A21" s="179" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="172"/>
-      <c r="C21" s="172"/>
-      <c r="D21" s="172"/>
-      <c r="E21" s="173"/>
+      <c r="B21" s="180"/>
+      <c r="C21" s="180"/>
+      <c r="D21" s="180"/>
+      <c r="E21" s="181"/>
     </row>
     <row r="22" spans="1:5" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="63" t="s">
@@ -4836,13 +5072,13 @@
       </c>
     </row>
     <row r="25" spans="1:5" s="16" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="171" t="s">
+      <c r="A25" s="179" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="172"/>
-      <c r="C25" s="172"/>
-      <c r="D25" s="172"/>
-      <c r="E25" s="173"/>
+      <c r="B25" s="180"/>
+      <c r="C25" s="180"/>
+      <c r="D25" s="180"/>
+      <c r="E25" s="181"/>
     </row>
     <row r="26" spans="1:5" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="63" t="s">
@@ -4888,13 +5124,13 @@
       </c>
     </row>
     <row r="29" spans="1:5" s="16" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="171" t="s">
+      <c r="A29" s="179" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="172"/>
-      <c r="C29" s="172"/>
-      <c r="D29" s="172"/>
-      <c r="E29" s="173"/>
+      <c r="B29" s="180"/>
+      <c r="C29" s="180"/>
+      <c r="D29" s="180"/>
+      <c r="E29" s="181"/>
     </row>
     <row r="30" spans="1:5" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="63" t="s">
@@ -4942,21 +5178,21 @@
       </c>
     </row>
     <row r="33" spans="1:5" s="16" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="162" t="s">
+      <c r="A33" s="170" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="163"/>
-      <c r="C33" s="163"/>
-      <c r="D33" s="163"/>
-      <c r="E33" s="164"/>
+      <c r="B33" s="171"/>
+      <c r="C33" s="171"/>
+      <c r="D33" s="171"/>
+      <c r="E33" s="172"/>
     </row>
     <row r="34" spans="1:5" s="16" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="168" t="s">
-        <v>76</v>
-      </c>
-      <c r="B34" s="169"/>
-      <c r="C34" s="169"/>
-      <c r="D34" s="170"/>
+      <c r="A34" s="176" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="177"/>
+      <c r="C34" s="177"/>
+      <c r="D34" s="178"/>
       <c r="E34" s="66">
         <f>SUM(E10:E12)+SUM(E14:E15)+SUM(E19:E20)+SUM(E23:E24)+SUM(E27:E28)+SUM(E31:E32)</f>
         <v>0</v>
@@ -4966,24 +5202,24 @@
       <c r="A35" s="49"/>
     </row>
     <row r="36" spans="1:5" s="16" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="A36" s="158" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" s="159"/>
-      <c r="C36" s="159"/>
-      <c r="D36" s="159"/>
+      <c r="A36" s="166" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="167"/>
+      <c r="C36" s="167"/>
+      <c r="D36" s="167"/>
       <c r="E36" s="91">
-        <f>'Budget Summary'!Q23</f>
+        <f>'Budget Summary'!X23</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="16" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="A37" s="160" t="s">
+      <c r="A37" s="168" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="161"/>
-      <c r="C37" s="161"/>
-      <c r="D37" s="161"/>
+      <c r="B37" s="169"/>
+      <c r="C37" s="169"/>
+      <c r="D37" s="169"/>
       <c r="E37" s="92">
         <f>E34-E36</f>
         <v>0</v>
@@ -5026,8 +5262,8 @@
   </sheetPr>
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -5418,70 +5654,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="10" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="173" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="167"/>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="175"/>
       <c r="F1" s="9"/>
       <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="176"/>
-      <c r="C2" s="156"/>
-      <c r="D2" s="156"/>
-      <c r="E2" s="157"/>
+        <v>76</v>
+      </c>
+      <c r="B2" s="184"/>
+      <c r="C2" s="164"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="165"/>
       <c r="I2" s="16"/>
     </row>
     <row r="3" spans="1:10" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="177" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3" s="178"/>
-      <c r="D3" s="178"/>
-      <c r="E3" s="179"/>
+      <c r="B3" s="185" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="186"/>
+      <c r="D3" s="186"/>
+      <c r="E3" s="187"/>
       <c r="F3" s="13"/>
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:10" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="51" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" s="176"/>
-      <c r="C4" s="156"/>
-      <c r="D4" s="156"/>
-      <c r="E4" s="157"/>
+        <v>84</v>
+      </c>
+      <c r="B4" s="184"/>
+      <c r="C4" s="164"/>
+      <c r="D4" s="164"/>
+      <c r="E4" s="165"/>
       <c r="I4" s="16"/>
     </row>
     <row r="5" spans="1:10" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="188" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="189"/>
-      <c r="D5" s="189"/>
-      <c r="E5" s="190"/>
+      <c r="B5" s="196" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="197"/>
+      <c r="D5" s="197"/>
+      <c r="E5" s="198"/>
       <c r="F5" s="13"/>
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:10" s="15" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="183"/>
-      <c r="C6" s="183"/>
-      <c r="D6" s="183"/>
-      <c r="E6" s="184"/>
+        <v>61</v>
+      </c>
+      <c r="B6" s="191"/>
+      <c r="C6" s="191"/>
+      <c r="D6" s="191"/>
+      <c r="E6" s="192"/>
       <c r="I6" s="16"/>
     </row>
     <row r="7" spans="1:10" ht="9" customHeight="1" x14ac:dyDescent="0.4">
@@ -5601,13 +5837,13 @@
       </c>
     </row>
     <row r="16" spans="1:10" s="16" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="171" t="s">
+      <c r="A16" s="179" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="172"/>
-      <c r="C16" s="172"/>
-      <c r="D16" s="172"/>
-      <c r="E16" s="173"/>
+      <c r="B16" s="180"/>
+      <c r="C16" s="180"/>
+      <c r="D16" s="180"/>
+      <c r="E16" s="181"/>
     </row>
     <row r="17" spans="1:5" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="62" t="s">
@@ -5674,13 +5910,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" s="16" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="171" t="s">
+      <c r="A21" s="179" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="172"/>
-      <c r="C21" s="172"/>
-      <c r="D21" s="172"/>
-      <c r="E21" s="173"/>
+      <c r="B21" s="180"/>
+      <c r="C21" s="180"/>
+      <c r="D21" s="180"/>
+      <c r="E21" s="181"/>
     </row>
     <row r="22" spans="1:5" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="63" t="s">
@@ -5732,13 +5968,13 @@
       </c>
     </row>
     <row r="25" spans="1:5" s="16" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="171" t="s">
+      <c r="A25" s="179" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="172"/>
-      <c r="C25" s="172"/>
-      <c r="D25" s="172"/>
-      <c r="E25" s="173"/>
+      <c r="B25" s="180"/>
+      <c r="C25" s="180"/>
+      <c r="D25" s="180"/>
+      <c r="E25" s="181"/>
     </row>
     <row r="26" spans="1:5" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="63" t="s">
@@ -5790,13 +6026,13 @@
       </c>
     </row>
     <row r="29" spans="1:5" s="16" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="171" t="s">
+      <c r="A29" s="179" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="172"/>
-      <c r="C29" s="172"/>
-      <c r="D29" s="172"/>
-      <c r="E29" s="173"/>
+      <c r="B29" s="180"/>
+      <c r="C29" s="180"/>
+      <c r="D29" s="180"/>
+      <c r="E29" s="181"/>
     </row>
     <row r="30" spans="1:5" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="63" t="s">
@@ -5848,33 +6084,33 @@
       </c>
     </row>
     <row r="33" spans="1:6" s="16" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="162" t="s">
+      <c r="A33" s="170" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="163"/>
-      <c r="C33" s="163"/>
-      <c r="D33" s="163"/>
-      <c r="E33" s="164"/>
+      <c r="B33" s="171"/>
+      <c r="C33" s="171"/>
+      <c r="D33" s="171"/>
+      <c r="E33" s="172"/>
     </row>
     <row r="34" spans="1:6" s="16" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="180" t="s">
-        <v>87</v>
-      </c>
-      <c r="B34" s="181"/>
-      <c r="C34" s="181"/>
-      <c r="D34" s="182"/>
+      <c r="A34" s="188" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="189"/>
+      <c r="C34" s="189"/>
+      <c r="D34" s="190"/>
       <c r="E34" s="103">
-        <f>'Budget Summary'!Q23*50%</f>
+        <f>'Budget Summary'!X23*100%</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="16" customFormat="1" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="185" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="186"/>
-      <c r="C35" s="186"/>
-      <c r="D35" s="187"/>
+      <c r="A35" s="193" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="194"/>
+      <c r="C35" s="194"/>
+      <c r="D35" s="195"/>
       <c r="E35" s="102">
         <f>SUM(E10:E12)+SUM(E14:E15)+SUM(E19:E20)+SUM(E23:E24)+SUM(E27:E28)+SUM(E31:E32)</f>
         <v>0</v>
@@ -5884,24 +6120,24 @@
       <c r="A36" s="49"/>
     </row>
     <row r="37" spans="1:6" s="16" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="A37" s="158" t="s">
-        <v>48</v>
-      </c>
-      <c r="B37" s="159"/>
-      <c r="C37" s="159"/>
-      <c r="D37" s="159"/>
+      <c r="A37" s="166" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" s="167"/>
+      <c r="C37" s="167"/>
+      <c r="D37" s="167"/>
       <c r="E37" s="91">
-        <f>'Budget Summary'!H23+'Budget Summary'!O23</f>
+        <f>'Budget Summary'!H23+'Budget Summary'!O23+'Budget Summary'!V23</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="16" customFormat="1" ht="13.9" x14ac:dyDescent="0.4">
-      <c r="A38" s="160" t="s">
+      <c r="A38" s="168" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="161"/>
-      <c r="C38" s="161"/>
-      <c r="D38" s="161"/>
+      <c r="B38" s="169"/>
+      <c r="C38" s="169"/>
+      <c r="D38" s="169"/>
       <c r="E38" s="92">
         <f>E35-E37</f>
         <v>0</v>
@@ -5910,23 +6146,23 @@
     <row r="39" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="40" spans="1:6" s="16" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A40" s="104" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B40" s="105"/>
       <c r="C40" s="105"/>
       <c r="D40" s="105"/>
       <c r="E40" s="105"/>
-      <c r="F40" s="191"/>
+      <c r="F40" s="111"/>
     </row>
     <row r="41" spans="1:6" s="16" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
-      <c r="A41" s="192" t="s">
-        <v>89</v>
-      </c>
-      <c r="B41" s="191"/>
-      <c r="C41" s="191"/>
-      <c r="D41" s="191"/>
-      <c r="E41" s="191"/>
-      <c r="F41" s="191"/>
+      <c r="A41" s="112" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="111"/>
+      <c r="C41" s="111"/>
+      <c r="D41" s="111"/>
+      <c r="E41" s="111"/>
+      <c r="F41" s="111"/>
     </row>
     <row r="42" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>

</xml_diff>